<commit_message>
finishing adding the measures to output excel file
</commit_message>
<xml_diff>
--- a/sonarqube-reports/linux-sonar-test/linux-sonar-test_master.xlsx
+++ b/sonarqube-reports/linux-sonar-test/linux-sonar-test_master.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Total</t>
   </si>
@@ -60,16 +60,28 @@
     <t>project measures</t>
   </si>
   <si>
+    <t>complexity</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>cognitive_complexity</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>ncloc</t>
   </si>
   <si>
+    <t>42</t>
+  </si>
+  <si>
     <t>comment_lines_density</t>
   </si>
   <si>
-    <t>complexity</t>
-  </si>
-  <si>
-    <t>cognitive_complexity</t>
+    <t>10.6</t>
   </si>
   <si>
     <t>measures</t>
@@ -109,9 +121,6 @@
   </si>
   <si>
     <t>unresolved issue</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>cpp:S1003</t>
@@ -549,9 +558,6 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="25.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="1:5">
       <c r="B2" s="1" t="s">
@@ -648,60 +654,76 @@
       <c r="E9" s="4"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="A12:D13"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -716,20 +738,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -752,124 +774,124 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>